<commit_message>
Oppdaterte kalenderen med oversiktsforelesning 25.08
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-H25.xlsx
+++ b/diverse/tidsplan-H25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C12A04-F43A-4D08-994A-466CECAE9848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAA9B0E-B156-48AC-8F49-4D53032E59D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1635" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>21.08:**Introduksjon til R** i Aud A</t>
   </si>
   <si>
-    <t>25.08: **Kontakttime** i Aud A</t>
-  </si>
-  <si>
     <t>01.09: (Ingen aktivitet)</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>13.11: Kontakttime, Aud A</t>
+  </si>
+  <si>
+    <t>25.08: **Oversiktsforelesning Grunnleggende statistikk** i Aud A</t>
   </si>
 </sst>
 </file>
@@ -491,17 +491,17 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +515,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>34</v>
       </c>
@@ -529,7 +529,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>35</v>
       </c>
@@ -537,13 +537,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>36</v>
       </c>
@@ -551,13 +551,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>37</v>
       </c>
@@ -565,14 +565,14 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>38</v>
       </c>
@@ -580,13 +580,13 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>39</v>
       </c>
@@ -594,14 +594,14 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>40</v>
       </c>
@@ -609,14 +609,14 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>41</v>
       </c>
@@ -624,13 +624,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>42</v>
       </c>
@@ -638,13 +638,13 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>43</v>
       </c>
@@ -652,13 +652,13 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>44</v>
       </c>
@@ -666,13 +666,13 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>45</v>
       </c>
@@ -680,13 +680,13 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>46</v>
       </c>
@@ -694,10 +694,10 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
en liten oppdatering i kalenderen
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-H25.xlsx
+++ b/diverse/tidsplan-H25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAA9B0E-B156-48AC-8F49-4D53032E59D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6661EA33-81D0-49F7-AC9A-AADCC3FE1A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>21.08:**Introduksjon til R** i Aud A</t>
   </si>
   <si>
-    <t>01.09: (Ingen aktivitet)</t>
-  </si>
-  <si>
     <t>08.09: **Oversiktsforelesning: Hypotesetesting** i Aud A</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>10.11: (Ingen aktivitet)</t>
   </si>
   <si>
-    <t>28.08: **Oppgaveseminar 1** i Aud A. Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
     <t>04.09: **Kontakttime** i Aud A</t>
   </si>
   <si>
@@ -151,6 +145,12 @@
   </si>
   <si>
     <t>25.08: **Oversiktsforelesning Grunnleggende statistikk** i Aud A</t>
+  </si>
+  <si>
+    <t>01.09: **Oppgaveseminar 1** i Aud A. Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>28.08: (Ingen aktivitet)</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,10 +537,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -551,10 +551,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -565,10 +565,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -580,10 +580,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -594,10 +594,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -609,10 +609,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -624,10 +624,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -638,10 +638,10 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -652,10 +652,10 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -666,10 +666,10 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -680,10 +680,10 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -694,10 +694,10 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
liten typo i kalender
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-H25.xlsx
+++ b/diverse/tidsplan-H25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BD669A-717A-4569-9198-F62CD41BE07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076A2792-5EE0-48EC-95F2-45284251740E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,7 +150,7 @@
     <t>28.08: (Ingen aktivitet)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 03.11: Praktisk informasjon om eksamen</t>
+    <t xml:space="preserve"> 03.11: Praktisk informasjon om eksamen i Aud A</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>